<commit_message>
Use jupyter notebook to run, not vscode
</commit_message>
<xml_diff>
--- a/pareto/jupyter_notebooks/strategic_model_general_demo/strategic_optimization_results.xlsx
+++ b/pareto/jupyter_notebooks/strategic_model_general_demo/strategic_optimization_results.xlsx
@@ -66062,7 +66062,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>74.79</t>
+          <t>68.56</t>
         </is>
       </c>
     </row>
@@ -66074,7 +66074,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>74.79</t>
+          <t>68.56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Try running jupyter notebook again
</commit_message>
<xml_diff>
--- a/pareto/jupyter_notebooks/strategic_model_general_demo/strategic_optimization_results.xlsx
+++ b/pareto/jupyter_notebooks/strategic_model_general_demo/strategic_optimization_results.xlsx
@@ -66062,7 +66062,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>68.56</t>
+          <t>67.6</t>
         </is>
       </c>
     </row>
@@ -66074,7 +66074,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>68.56</t>
+          <t>67.59</t>
         </is>
       </c>
     </row>

</xml_diff>